<commit_message>
format lại dữ liệu export
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Sales_Order_By_Employee_And_Item.xlsx
+++ b/DMS/Templates/Report_Sales_Order_By_Employee_And_Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE41C64-77CD-447A-9D6B-A003F96CD632}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164FEAD5-70B9-48EB-82DA-1133D712B729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>BÁO CÁO BÁN HÀNG THEO NHÂN VIÊN VÀ SẢN PHẨM</t>
   </si>
   <si>
-    <t>Số cửa hàng mua</t>
-  </si>
-  <si>
     <t>CÔNG TY CỔ PHẦN BÓNG ĐÈN PHÍCH NƯỚC RẠNG ĐÔNG</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>{{Total.TotalRevenue}}</t>
+  </si>
+  <si>
+    <t>Số đại lý mua</t>
   </si>
 </sst>
 </file>
@@ -294,6 +294,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -324,17 +327,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,103 +619,103 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="5.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="3" customWidth="1"/>
+    <col min="1" max="3" width="5.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="20" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="14" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="15" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="3"/>
+    <col min="15" max="15" width="15.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
-    <row r="4" spans="1:16" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,97 +744,97 @@
         <v>11</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="12"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" s="17" t="s">
+    <row r="10" spans="1:16" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="19" t="s">
+      <c r="K10" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>35</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>

</xml_diff>

<commit_message>
thêm báo cáo bán hàng theo đơn trực tiếp
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Sales_Order_By_Employee_And_Item.xlsx
+++ b/DMS/Templates/Report_Sales_Order_By_Employee_And_Item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164FEAD5-70B9-48EB-82DA-1133D712B729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0168A05E-03BB-4603-AC53-B5FCB70114F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Items.BuyerStoreCounter}}</t>
   </si>
   <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Items.IndirectSalesOrderCounter}}</t>
-  </si>
-  <si>
     <t>{{Total.TotalSalesStock}}</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Số đại lý mua</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Items.SalesOrderCounter}}</t>
   </si>
 </sst>
 </file>
@@ -297,6 +297,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -326,15 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,7 +619,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,47 +642,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -704,18 +704,18 @@
       <c r="L5" s="4"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,42 +744,42 @@
         <v>11</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="20"/>
+      <c r="E9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
@@ -789,52 +789,52 @@
       <c r="I9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="19" t="s">
+      <c r="O9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="20" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="L10" s="6"/>
+      <c r="M10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="20" t="s">
+      <c r="N10" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>

</xml_diff>